<commit_message>
feat(word_files): reading and wrintg word files
</commit_message>
<xml_diff>
--- a/book_questions/chapter_12/examples.xlsx
+++ b/book_questions/chapter_12/examples.xlsx
@@ -4,26 +4,46 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Spam Bacon Eggs Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <sz val="24"/>
     </font>
   </fonts>
   <fills count="2">
@@ -43,16 +63,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -409,18 +449,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <cols>
+    <col width="20" customWidth="1" style="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="70" customHeight="1" s="2">
+      <c r="A1" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1">
+        <f>SOMA(A1:C1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="2">
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>Mesclar</t>
+        </is>
+      </c>
+    </row>
+    <row r="4"/>
+    <row r="5"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:C5"/>
+  </mergeCells>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
</xml_diff>